<commit_message>
Woche 1 Resultat Kreuz und Schriftzug vorhanden
</commit_message>
<xml_diff>
--- a/res/Zeitplanung.xlsx
+++ b/res/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidadmin\Documents\ICT_BZ\Mein_Projekt\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D623A780-284E-4637-8BAF-0EF2D68D35DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAA0661-F60C-4ECF-97E1-F6A6342A9390}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12950" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1079,7 +1079,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1414,10 +1414,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1525,7 +1521,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14</c:v>
@@ -1599,7 +1595,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2107,8 +2103,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AK39" sqref="AK39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2979,14 +2975,14 @@
       <c r="AQ12" s="60"/>
       <c r="AR12" s="61"/>
       <c r="AS12" s="61"/>
-      <c r="AT12" s="63"/>
+      <c r="AT12" s="56"/>
       <c r="AU12" s="57"/>
       <c r="AV12" s="58"/>
       <c r="AW12" s="59"/>
       <c r="AX12" s="60"/>
       <c r="AY12" s="61"/>
       <c r="AZ12" s="61"/>
-      <c r="BA12" s="63"/>
+      <c r="BA12" s="56"/>
       <c r="BB12" s="57"/>
       <c r="BC12" s="58"/>
       <c r="BD12" s="59"/>
@@ -3052,7 +3048,7 @@
       <c r="AP13" s="59"/>
       <c r="AQ13" s="60"/>
       <c r="AR13" s="55"/>
-      <c r="AS13" s="100"/>
+      <c r="AS13" s="87"/>
       <c r="AT13" s="55"/>
       <c r="AU13" s="66"/>
       <c r="AV13" s="67"/>
@@ -3066,7 +3062,6 @@
       <c r="BD13" s="59"/>
       <c r="BE13" s="60"/>
       <c r="BF13" s="55"/>
-      <c r="BG13" s="87"/>
       <c r="BH13" s="55"/>
       <c r="BI13" s="66"/>
       <c r="BJ13" s="67"/>
@@ -3374,11 +3369,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3450,8 +3445,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="83">
-        <f>SUM(G19:BJ19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="50">
         <v>1</v>
@@ -3522,11 +3516,10 @@
         <v>48</v>
       </c>
       <c r="C20" s="49">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20" s="83">
-        <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3600,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="83">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D21:D30" si="0">SUM(G21:BJ21)</f>
         <v>0</v>
       </c>
       <c r="E21" s="50">
@@ -3675,8 +3668,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3795,8 +3787,7 @@
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
       <c r="AR23" s="63"/>
-      <c r="AS23" s="63"/>
-      <c r="AT23" s="87"/>
+      <c r="AS23" s="87"/>
       <c r="AU23" s="57"/>
       <c r="AV23" s="58"/>
       <c r="AW23" s="59"/>
@@ -3870,8 +3861,7 @@
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
       <c r="AR24" s="90"/>
-      <c r="AS24" s="90"/>
-      <c r="AT24" s="63"/>
+      <c r="AS24" s="63"/>
       <c r="AU24" s="57"/>
       <c r="AV24" s="58"/>
       <c r="AW24" s="59"/>
@@ -4388,7 +4378,6 @@
         <v>2</v>
       </c>
       <c r="D32" s="83">
-        <f>SUM(G32:BJ32)</f>
         <v>0</v>
       </c>
       <c r="E32" s="50"/>
@@ -5175,11 +5164,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5507,11 +5496,11 @@
       <c r="B5" s="97"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Endprodukt Woche 2 Snake läuft 1 Feld Knopf Funktioniert nicht
</commit_message>
<xml_diff>
--- a/res/Zeitplanung.xlsx
+++ b/res/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidadmin\Documents\ICT_BZ\Mein_Projekt\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82D6DD6-41E3-40D9-AF96-4B87671C1699}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5B9032-1FF0-4383-AEAC-138BD162C5CE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12950" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1389,6 +1389,14 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1419,14 +1427,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1602,7 +1602,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.5</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -2116,8 +2116,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2436,88 +2436,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="91"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="93"/>
-      <c r="N7" s="92" t="s">
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="92"/>
-      <c r="P7" s="92"/>
-      <c r="Q7" s="92"/>
-      <c r="R7" s="92"/>
-      <c r="S7" s="92"/>
-      <c r="T7" s="93"/>
-      <c r="U7" s="92" t="s">
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="94"/>
+      <c r="T7" s="95"/>
+      <c r="U7" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92"/>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="93"/>
-      <c r="AB7" s="94" t="s">
+      <c r="V7" s="94"/>
+      <c r="W7" s="94"/>
+      <c r="X7" s="94"/>
+      <c r="Y7" s="94"/>
+      <c r="Z7" s="94"/>
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="92"/>
-      <c r="AD7" s="92"/>
-      <c r="AE7" s="92"/>
-      <c r="AF7" s="92"/>
-      <c r="AG7" s="92"/>
-      <c r="AH7" s="93"/>
-      <c r="AI7" s="92" t="s">
+      <c r="AC7" s="94"/>
+      <c r="AD7" s="94"/>
+      <c r="AE7" s="94"/>
+      <c r="AF7" s="94"/>
+      <c r="AG7" s="94"/>
+      <c r="AH7" s="95"/>
+      <c r="AI7" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="92"/>
-      <c r="AK7" s="92"/>
-      <c r="AL7" s="92"/>
-      <c r="AM7" s="92"/>
-      <c r="AN7" s="92"/>
-      <c r="AO7" s="93"/>
-      <c r="AP7" s="94" t="s">
+      <c r="AJ7" s="94"/>
+      <c r="AK7" s="94"/>
+      <c r="AL7" s="94"/>
+      <c r="AM7" s="94"/>
+      <c r="AN7" s="94"/>
+      <c r="AO7" s="95"/>
+      <c r="AP7" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="92"/>
-      <c r="AR7" s="92"/>
-      <c r="AS7" s="92"/>
-      <c r="AT7" s="92"/>
-      <c r="AU7" s="92"/>
-      <c r="AV7" s="93"/>
-      <c r="AW7" s="92" t="s">
+      <c r="AQ7" s="94"/>
+      <c r="AR7" s="94"/>
+      <c r="AS7" s="94"/>
+      <c r="AT7" s="94"/>
+      <c r="AU7" s="94"/>
+      <c r="AV7" s="95"/>
+      <c r="AW7" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="92"/>
-      <c r="AY7" s="92"/>
-      <c r="AZ7" s="92"/>
-      <c r="BA7" s="92"/>
-      <c r="BB7" s="92"/>
-      <c r="BC7" s="93"/>
-      <c r="BD7" s="94" t="s">
+      <c r="AX7" s="94"/>
+      <c r="AY7" s="94"/>
+      <c r="AZ7" s="94"/>
+      <c r="BA7" s="94"/>
+      <c r="BB7" s="94"/>
+      <c r="BC7" s="95"/>
+      <c r="BD7" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="BE7" s="92"/>
-      <c r="BF7" s="92"/>
-      <c r="BG7" s="92"/>
-      <c r="BH7" s="92"/>
-      <c r="BI7" s="92"/>
-      <c r="BJ7" s="95"/>
+      <c r="BE7" s="94"/>
+      <c r="BF7" s="94"/>
+      <c r="BG7" s="94"/>
+      <c r="BH7" s="94"/>
+      <c r="BI7" s="94"/>
+      <c r="BJ7" s="97"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2968,7 +2968,9 @@
       <c r="O12" s="60"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="63"/>
+      <c r="R12" s="63">
+        <v>0.6</v>
+      </c>
       <c r="S12" s="57"/>
       <c r="T12" s="58"/>
       <c r="U12" s="59"/>
@@ -3814,18 +3816,18 @@
       <c r="Y23" s="63"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
-      <c r="AB23" s="100"/>
-      <c r="AC23" s="101"/>
-      <c r="AD23" s="101"/>
-      <c r="AE23" s="101"/>
-      <c r="AF23" s="101"/>
+      <c r="AB23" s="91"/>
+      <c r="AC23" s="92"/>
+      <c r="AD23" s="92"/>
+      <c r="AE23" s="92"/>
+      <c r="AF23" s="92"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="58"/>
-      <c r="AI23" s="100"/>
-      <c r="AJ23" s="101"/>
-      <c r="AK23" s="101"/>
-      <c r="AL23" s="101"/>
-      <c r="AM23" s="101"/>
+      <c r="AI23" s="91"/>
+      <c r="AJ23" s="92"/>
+      <c r="AK23" s="92"/>
+      <c r="AL23" s="92"/>
+      <c r="AM23" s="92"/>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
@@ -5212,7 +5214,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>20.5</v>
+        <v>21.1</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5262,7 +5264,7 @@
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="S43" s="39">
         <f t="shared" si="3"/>
@@ -5487,10 +5489,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5499,28 +5501,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="96" t="str">
+      <c r="A3" s="98" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="97"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>7</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="96" t="str">
+      <c r="A4" s="98" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>12</v>
@@ -5533,11 +5535,11 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="96" t="str">
+      <c r="A5" s="98" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="97"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>45</v>
@@ -5550,11 +5552,11 @@
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="96" t="str">
+      <c r="A6" s="98" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="97"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>14</v>
@@ -5566,11 +5568,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="96" t="str">
+      <c r="A7" s="98" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>8</v>
@@ -5582,11 +5584,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="96" t="str">
+      <c r="A8" s="98" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="97"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>0</v>

</xml_diff>

<commit_message>
Etwas mit dem Drehgeber herzmgespielt
</commit_message>
<xml_diff>
--- a/res/Zeitplanung.xlsx
+++ b/res/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidadmin\Documents\ICT_BZ\Mein_Projekt\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CDA9EB-82DE-4FD3-8B9F-0DD586F1BA96}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39204C24-E479-49FC-AE48-F941339AF5FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12950" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1608,7 +1608,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2117,7 +2117,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E23" s="50">
         <v>1</v>
@@ -3815,7 +3815,9 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="63"/>
+      <c r="W23" s="63">
+        <v>8</v>
+      </c>
       <c r="X23" s="63"/>
       <c r="Y23" s="63"/>
       <c r="Z23" s="57"/>
@@ -5218,7 +5220,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>34.1</v>
+        <v>42.1</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5288,7 +5290,7 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
@@ -5550,7 +5552,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Zeitplanung aktualiert Snake bei neustart auf rechts END nicht mehr Farbig
</commit_message>
<xml_diff>
--- a/res/Zeitplanung.xlsx
+++ b/res/Zeitplanung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidadmin\Documents\ICT_BZ\Mein_Projekt\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidadmin\Documents\ICT_BZ\Wortuhr_Snake\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FDE3FE-18B5-4056-A626-2051E95E96F4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0ACFDBB-EF99-4517-9ADD-88C446246B45}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12950" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="56">
   <si>
     <t>Nr.</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>Bugs fixen</t>
-  </si>
-  <si>
-    <t>Testfälle durchführen + dokumentieren</t>
   </si>
   <si>
     <t>Reserve</t>
@@ -232,6 +229,12 @@
   </si>
   <si>
     <t>Keine Verzögerungen beim System</t>
+  </si>
+  <si>
+    <t>Testfälle durchführen</t>
+  </si>
+  <si>
+    <t>Abschlussbericht</t>
   </si>
 </sst>
 </file>
@@ -340,7 +343,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,11 +438,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FF92D050"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="49">
     <border>
@@ -1084,7 +1082,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1386,14 +1384,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1543,7 +1533,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1602,22 +1592,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.0999999999999996</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2116,8 +2106,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AF24" sqref="AF24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2133,7 +2123,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2238,7 +2228,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="86"/>
       <c r="H3" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2368,7 +2358,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="6"/>
@@ -2436,88 +2426,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="93"/>
+      <c r="D7" s="91"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="93"/>
+      <c r="N7" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="94" t="s">
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="92"/>
+      <c r="S7" s="92"/>
+      <c r="T7" s="93"/>
+      <c r="U7" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="95"/>
-      <c r="U7" s="94" t="s">
+      <c r="V7" s="92"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="92"/>
+      <c r="Y7" s="92"/>
+      <c r="Z7" s="92"/>
+      <c r="AA7" s="93"/>
+      <c r="AB7" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="94"/>
-      <c r="W7" s="94"/>
-      <c r="X7" s="94"/>
-      <c r="Y7" s="94"/>
-      <c r="Z7" s="94"/>
-      <c r="AA7" s="95"/>
-      <c r="AB7" s="96" t="s">
+      <c r="AC7" s="92"/>
+      <c r="AD7" s="92"/>
+      <c r="AE7" s="92"/>
+      <c r="AF7" s="92"/>
+      <c r="AG7" s="92"/>
+      <c r="AH7" s="93"/>
+      <c r="AI7" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="94"/>
-      <c r="AD7" s="94"/>
-      <c r="AE7" s="94"/>
-      <c r="AF7" s="94"/>
-      <c r="AG7" s="94"/>
-      <c r="AH7" s="95"/>
-      <c r="AI7" s="94" t="s">
+      <c r="AJ7" s="92"/>
+      <c r="AK7" s="92"/>
+      <c r="AL7" s="92"/>
+      <c r="AM7" s="92"/>
+      <c r="AN7" s="92"/>
+      <c r="AO7" s="93"/>
+      <c r="AP7" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="94"/>
-      <c r="AK7" s="94"/>
-      <c r="AL7" s="94"/>
-      <c r="AM7" s="94"/>
-      <c r="AN7" s="94"/>
-      <c r="AO7" s="95"/>
-      <c r="AP7" s="96" t="s">
+      <c r="AQ7" s="92"/>
+      <c r="AR7" s="92"/>
+      <c r="AS7" s="92"/>
+      <c r="AT7" s="92"/>
+      <c r="AU7" s="92"/>
+      <c r="AV7" s="93"/>
+      <c r="AW7" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="94"/>
-      <c r="AR7" s="94"/>
-      <c r="AS7" s="94"/>
-      <c r="AT7" s="94"/>
-      <c r="AU7" s="94"/>
-      <c r="AV7" s="95"/>
-      <c r="AW7" s="94" t="s">
+      <c r="AX7" s="92"/>
+      <c r="AY7" s="92"/>
+      <c r="AZ7" s="92"/>
+      <c r="BA7" s="92"/>
+      <c r="BB7" s="92"/>
+      <c r="BC7" s="93"/>
+      <c r="BD7" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="94"/>
-      <c r="AY7" s="94"/>
-      <c r="AZ7" s="94"/>
-      <c r="BA7" s="94"/>
-      <c r="BB7" s="94"/>
-      <c r="BC7" s="95"/>
-      <c r="BD7" s="96" t="s">
-        <v>42</v>
-      </c>
-      <c r="BE7" s="94"/>
-      <c r="BF7" s="94"/>
-      <c r="BG7" s="94"/>
-      <c r="BH7" s="94"/>
-      <c r="BI7" s="94"/>
-      <c r="BJ7" s="97"/>
+      <c r="BE7" s="92"/>
+      <c r="BF7" s="92"/>
+      <c r="BG7" s="92"/>
+      <c r="BH7" s="92"/>
+      <c r="BI7" s="92"/>
+      <c r="BJ7" s="95"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
@@ -2534,7 +2524,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>16</v>
@@ -2718,7 +2708,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2787,7 +2777,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="84">
         <f>SUM(G10:BJ10)</f>
@@ -2797,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2861,14 +2851,14 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="49">
         <v>2</v>
       </c>
       <c r="D11" s="83">
         <f>SUM(G11:BJ11)</f>
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2877,7 +2867,7 @@
       <c r="G11" s="59"/>
       <c r="H11" s="60"/>
       <c r="I11" s="61">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="J11" s="87"/>
       <c r="K11" s="85"/>
@@ -2898,7 +2888,9 @@
       <c r="V11" s="60"/>
       <c r="W11" s="61"/>
       <c r="X11" s="61"/>
-      <c r="Y11" s="56"/>
+      <c r="Y11" s="56">
+        <v>1</v>
+      </c>
       <c r="Z11" s="57"/>
       <c r="AA11" s="58"/>
       <c r="AB11" s="59"/>
@@ -2919,7 +2911,9 @@
       <c r="AQ11" s="60"/>
       <c r="AR11" s="61"/>
       <c r="AS11" s="61"/>
-      <c r="AT11" s="56"/>
+      <c r="AT11" s="56">
+        <v>1.5</v>
+      </c>
       <c r="AU11" s="57"/>
       <c r="AV11" s="58"/>
       <c r="AW11" s="59"/>
@@ -2949,7 +2943,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3000,7 +2994,9 @@
       <c r="AQ12" s="60"/>
       <c r="AR12" s="61"/>
       <c r="AS12" s="61"/>
-      <c r="AT12" s="56"/>
+      <c r="AT12" s="63">
+        <v>1</v>
+      </c>
       <c r="AU12" s="57"/>
       <c r="AV12" s="58"/>
       <c r="AW12" s="59"/>
@@ -3023,10 +3019,10 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="83">
         <f>SUM(G13:BJ13)</f>
@@ -3036,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3107,7 +3103,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3173,27 +3169,29 @@
         <v>201</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="49">
         <v>4</v>
       </c>
       <c r="D15" s="83">
         <f>SUM(G15:BJ15)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="50">
         <v>1</v>
       </c>
       <c r="F15" s="89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
       <c r="I15" s="68">
-        <v>3</v>
-      </c>
-      <c r="J15" s="87"/>
+        <v>4</v>
+      </c>
+      <c r="J15" s="87">
+        <v>1</v>
+      </c>
       <c r="K15" s="90"/>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
@@ -3252,14 +3250,14 @@
         <v>202</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="49">
         <v>8</v>
       </c>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="50">
         <v>1</v>
@@ -3273,7 +3271,9 @@
       <c r="J16" s="68">
         <v>3</v>
       </c>
-      <c r="K16" s="56"/>
+      <c r="K16" s="56">
+        <v>2</v>
+      </c>
       <c r="L16" s="57"/>
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3474,14 +3474,14 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="49">
         <v>2</v>
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E19" s="50">
         <v>1</v>
@@ -3490,8 +3490,12 @@
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
       <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="56"/>
+      <c r="J19" s="55">
+        <v>2</v>
+      </c>
+      <c r="K19" s="56">
+        <v>2</v>
+      </c>
       <c r="L19" s="57"/>
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
@@ -3551,14 +3555,14 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="49">
         <v>6</v>
       </c>
       <c r="D20" s="83">
         <f>SUM(G20:BJ20)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3567,14 +3571,18 @@
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="J20" s="55">
+        <v>2</v>
+      </c>
+      <c r="K20" s="56">
+        <v>3</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
       <c r="P20" s="63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q20" s="63">
         <v>0</v>
@@ -3630,7 +3638,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="49">
         <v>0</v>
@@ -3705,7 +3713,7 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="49">
         <v>3</v>
@@ -3784,14 +3792,14 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="49">
         <v>30</v>
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E23" s="50">
         <v>1</v>
@@ -3808,7 +3816,7 @@
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
       <c r="Q23" s="90">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R23" s="90">
         <v>7</v>
@@ -3818,34 +3826,39 @@
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
       <c r="W23" s="63">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X23" s="63">
         <v>8</v>
       </c>
       <c r="Y23" s="63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
-      <c r="AB23" s="91"/>
-      <c r="AC23" s="92"/>
-      <c r="AD23" s="92"/>
-      <c r="AE23" s="92"/>
-      <c r="AF23" s="92"/>
+      <c r="AB23" s="53"/>
+      <c r="AC23" s="54"/>
+      <c r="AD23" s="54"/>
+      <c r="AE23" s="54"/>
+      <c r="AF23" s="54"/>
       <c r="AG23" s="57"/>
       <c r="AH23" s="58"/>
-      <c r="AI23" s="91"/>
-      <c r="AJ23" s="92"/>
-      <c r="AK23" s="92"/>
-      <c r="AL23" s="92"/>
-      <c r="AM23" s="92"/>
+      <c r="AI23" s="53"/>
+      <c r="AJ23" s="54"/>
+      <c r="AK23" s="54"/>
+      <c r="AL23" s="54"/>
+      <c r="AM23" s="54"/>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="63"/>
-      <c r="AS23" s="87"/>
+      <c r="AR23" s="63">
+        <v>6</v>
+      </c>
+      <c r="AS23" s="63">
+        <v>2</v>
+      </c>
+      <c r="AT23" s="87"/>
       <c r="AU23" s="57"/>
       <c r="AV23" s="58"/>
       <c r="AW23" s="59"/>
@@ -3868,7 +3881,7 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="49">
         <v>4</v>
@@ -3919,7 +3932,9 @@
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
       <c r="AR24" s="90"/>
-      <c r="AS24" s="63"/>
+      <c r="AS24" s="63">
+        <v>0</v>
+      </c>
       <c r="AU24" s="57"/>
       <c r="AV24" s="58"/>
       <c r="AW24" s="59"/>
@@ -4364,7 +4379,7 @@
       </c>
       <c r="D31" s="42">
         <f>SUM(D32:D35)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="31"/>
@@ -4477,9 +4492,9 @@
       <c r="AO32" s="58"/>
       <c r="AP32" s="53"/>
       <c r="AQ32" s="54"/>
-      <c r="AR32" s="63"/>
+      <c r="AR32" s="55"/>
       <c r="AS32" s="55"/>
-      <c r="AT32" s="56"/>
+      <c r="AT32" s="63"/>
       <c r="AU32" s="57"/>
       <c r="AV32" s="58"/>
       <c r="AW32" s="53"/>
@@ -4502,14 +4517,14 @@
         <v>402</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C33" s="49">
         <v>4</v>
       </c>
       <c r="D33" s="83">
         <f t="shared" ref="D33:D35" si="1">SUM(G33:BJ33)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="50"/>
       <c r="F33" s="51"/>
@@ -4550,8 +4565,9 @@
       <c r="AO33" s="58"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="60"/>
-      <c r="AR33" s="63"/>
-      <c r="AS33" s="55"/>
+      <c r="AS33" s="63">
+        <v>1</v>
+      </c>
       <c r="AT33" s="56"/>
       <c r="AU33" s="57"/>
       <c r="AV33" s="58"/>
@@ -4582,7 +4598,7 @@
       </c>
       <c r="D34" s="83">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
@@ -4623,8 +4639,12 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="55"/>
-      <c r="AS34" s="63"/>
+      <c r="AR34" s="63">
+        <v>2</v>
+      </c>
+      <c r="AS34" s="63">
+        <v>3</v>
+      </c>
       <c r="AT34" s="63"/>
       <c r="AU34" s="57"/>
       <c r="AV34" s="58"/>
@@ -4791,7 +4811,7 @@
         <v>501</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="49">
         <v>8</v>
@@ -4937,11 +4957,11 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="31"/>
@@ -5007,7 +5027,7 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="49">
         <v>0</v>
@@ -5080,12 +5100,14 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="49"/>
+        <v>30</v>
+      </c>
+      <c r="C41" s="49">
+        <v>4</v>
+      </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E41" s="50"/>
       <c r="F41" s="51"/>
@@ -5127,8 +5149,12 @@
       <c r="AP41" s="59"/>
       <c r="AQ41" s="60"/>
       <c r="AR41" s="55"/>
-      <c r="AS41" s="55"/>
-      <c r="AT41" s="56"/>
+      <c r="AS41" s="55">
+        <v>2</v>
+      </c>
+      <c r="AT41" s="56">
+        <v>2</v>
+      </c>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
       <c r="AW41" s="59"/>
@@ -5150,11 +5176,15 @@
       <c r="A42" s="12">
         <v>603</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="49"/>
+      <c r="B42" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="49">
+        <v>1</v>
+      </c>
       <c r="D42" s="83">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="50"/>
       <c r="F42" s="51"/>
@@ -5197,7 +5227,9 @@
       <c r="AQ42" s="70"/>
       <c r="AR42" s="55"/>
       <c r="AS42" s="55"/>
-      <c r="AT42" s="56"/>
+      <c r="AT42" s="56">
+        <v>1</v>
+      </c>
       <c r="AU42" s="57"/>
       <c r="AV42" s="58"/>
       <c r="AW42" s="69"/>
@@ -5222,11 +5254,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>58.1</v>
+        <v>90.1</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5240,15 +5272,15 @@
       </c>
       <c r="I43" s="39">
         <f t="shared" si="3"/>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5268,11 +5300,11 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5296,7 +5328,7 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
@@ -5380,15 +5412,15 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AT43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="AU43" s="39">
         <f t="shared" si="4"/>
@@ -5486,8 +5518,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -5501,10 +5533,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5513,78 +5545,78 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="98" t="str">
+      <c r="A3" s="96" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="99"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>7</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>4.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="98" t="str">
+      <c r="A4" s="96" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="99"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>12</v>
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="98" t="str">
+      <c r="A5" s="96" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>45</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="98" t="str">
+      <c r="A6" s="96" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="99"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>14</v>
       </c>
       <c r="D6" s="80">
         <f>Zeitplanung!D31</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="98" t="str">
+      <c r="A7" s="96" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="99"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>8</v>
@@ -5596,18 +5628,18 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="98" t="str">
+      <c r="A8" s="96" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="99"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="81"/>
     </row>

</xml_diff>